<commit_message>
opt@3.0.1#:update sheets for 3.0.1
</commit_message>
<xml_diff>
--- a/VersionRecords/Version3.0.1/版本Bug和特性计划及评审表v3.0.1.xlsx
+++ b/VersionRecords/Version3.0.1/版本Bug和特性计划及评审表v3.0.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Test\Mogo_Doc\VersionRecords\Version3.0.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\mogo_git\Mogo_Doc\VersionRecords\Version3.0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="182">
   <si>
     <t>No</t>
   </si>
@@ -447,6 +447,249 @@
   </si>
   <si>
     <t>发现组</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>QQ在线客服时间更改+ 页脚</t>
+  </si>
+  <si>
+    <t>New Features</t>
+  </si>
+  <si>
+    <t>租客PC</t>
+  </si>
+  <si>
+    <t>裔玲玲</t>
+  </si>
+  <si>
+    <t>EQ组</t>
+  </si>
+  <si>
+    <t>吴永余</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试通过</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>能</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>”房东入驻“页面入口变更至房东pc登录页</t>
+  </si>
+  <si>
+    <t>李健</t>
+  </si>
+  <si>
+    <t>吴永余</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>频道更改 - header UI修改，城市切换</t>
+  </si>
+  <si>
+    <t>吴永余</t>
+  </si>
+  <si>
+    <t>官网首页“蘑菇客”公众号推广展示</t>
+  </si>
+  <si>
+    <t>陈佳文</t>
+  </si>
+  <si>
+    <t>测试通过</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>能</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>无图版本房间详情页优化</t>
+  </si>
+  <si>
+    <t>王龙国</t>
+  </si>
+  <si>
+    <t>官网首页资讯调取规则优化。将官网首页蘑菇资讯调用规则数据进行更改，改为调用社区的最新文章。</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>纪林强</t>
+  </si>
+  <si>
+    <t>集中式房源，电梯数为0，租客APP对应房间显示标签电梯房 （redmine: 45832）</t>
+  </si>
+  <si>
+    <t>BugFix</t>
+  </si>
+  <si>
+    <t>彭晓春</t>
+  </si>
+  <si>
+    <t>anna</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试通过</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>能</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>解决上线前老数据，账单实际已支付显示为未支付的问题</t>
+  </si>
+  <si>
+    <t>租客APP</t>
+  </si>
+  <si>
+    <t>周云</t>
+  </si>
+  <si>
+    <t>anna</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试通过</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>能</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>解决找房列表出现价格为0的问题</t>
+  </si>
+  <si>
+    <t>租客PC/租客APP</t>
+  </si>
+  <si>
+    <t>雷传盛</t>
+  </si>
+  <si>
+    <t>搜索引擎优化如果显示0 的数据 会自动同步showPrices 字段</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>官网，微官网 添加沪公网安备信息</t>
+  </si>
+  <si>
+    <t>anna</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>能</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>自营合同模版修改</t>
+  </si>
+  <si>
+    <t>金刚</t>
+  </si>
+  <si>
+    <t>anna</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>此定时器会修改 预定单是预定已支付待确认的状态 修改为 预定成功待审核
+签约单是 23 状态修改为 4</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>新增定时器：处理支付回掉失败</t>
+  </si>
+  <si>
+    <t>新增定时器：支付成功可再支付问题</t>
+  </si>
+  <si>
+    <t>冯银鹏</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>架构组</t>
+  </si>
+  <si>
+    <t>能</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加百度官方监测工具实时监测网站数据变化</t>
+  </si>
+  <si>
+    <t>找房添加地铁站找房</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>王龙国</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试中</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改租客PC安全中心页 -标签 BUG</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>EQ组</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>吴永余</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>房东PC 添加申请加盟按钮</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>房东PC</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>余星赞</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>余星赞</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>李敖</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>李敖</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>邵明基</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>能</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -454,7 +697,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -542,6 +785,29 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -563,7 +829,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -649,6 +915,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -670,7 +947,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -789,6 +1066,36 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="16" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1146,34 +1453,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="44.21875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="22.44140625" style="19" customWidth="1"/>
-    <col min="4" max="4" width="22.77734375" style="19" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" style="19" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" style="20" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" style="19" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="20" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" style="20" customWidth="1"/>
-    <col min="10" max="10" width="23.88671875" style="19" customWidth="1"/>
-    <col min="11" max="12" width="11.88671875" style="19" customWidth="1"/>
+    <col min="1" max="1" width="3.5" style="19" customWidth="1"/>
+    <col min="2" max="2" width="44.25" style="20" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="19" customWidth="1"/>
+    <col min="4" max="4" width="22.75" style="19" customWidth="1"/>
+    <col min="5" max="5" width="9.75" style="19" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="20" customWidth="1"/>
+    <col min="7" max="7" width="9.75" style="19" customWidth="1"/>
+    <col min="8" max="8" width="11.625" style="20" customWidth="1"/>
+    <col min="9" max="9" width="12.875" style="20" customWidth="1"/>
+    <col min="10" max="10" width="23.875" style="19" customWidth="1"/>
+    <col min="11" max="12" width="11.875" style="19" customWidth="1"/>
     <col min="13" max="13" width="9" style="20"/>
-    <col min="14" max="14" width="11.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" style="20" customWidth="1"/>
-    <col min="16" max="16" width="12.109375" style="23" customWidth="1"/>
-    <col min="17" max="18" width="17.6640625" style="23" customWidth="1"/>
-    <col min="19" max="19" width="48.44140625" style="20" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" customWidth="1"/>
+    <col min="14" max="14" width="11.625" style="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.625" style="20" customWidth="1"/>
+    <col min="16" max="16" width="12.125" style="23" customWidth="1"/>
+    <col min="17" max="18" width="17.625" style="23" customWidth="1"/>
+    <col min="19" max="19" width="48.5" style="20" customWidth="1"/>
+    <col min="20" max="20" width="8.875" customWidth="1"/>
     <col min="21" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="1" customFormat="1" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1232,7 +1539,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -1264,10 +1571,18 @@
       <c r="K2" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="14"/>
+      <c r="L2" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="N2" s="13">
+        <v>42436</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>181</v>
+      </c>
       <c r="P2" s="22">
         <v>1202</v>
       </c>
@@ -1278,7 +1593,7 @@
       <c r="S2" s="18"/>
       <c r="T2" s="10"/>
     </row>
-    <row r="3" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -1310,10 +1625,18 @@
       <c r="K3" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="14"/>
+      <c r="L3" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="N3" s="13">
+        <v>42436</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>181</v>
+      </c>
       <c r="P3" s="22">
         <v>1217</v>
       </c>
@@ -1324,7 +1647,7 @@
       <c r="S3" s="18"/>
       <c r="T3" s="10"/>
     </row>
-    <row r="4" spans="1:20" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" s="11" customFormat="1" ht="33" x14ac:dyDescent="0.35">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -1356,10 +1679,18 @@
       <c r="K4" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="14"/>
+      <c r="L4" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="N4" s="13">
+        <v>42436</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>181</v>
+      </c>
       <c r="P4" s="22">
         <v>827</v>
       </c>
@@ -1370,7 +1701,7 @@
       <c r="S4" s="18"/>
       <c r="T4" s="10"/>
     </row>
-    <row r="5" spans="1:20" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" s="11" customFormat="1" ht="33" x14ac:dyDescent="0.35">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -1402,10 +1733,18 @@
       <c r="K5" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="L5" s="12"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="14"/>
+      <c r="L5" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="N5" s="13">
+        <v>42436</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>181</v>
+      </c>
       <c r="P5" s="22">
         <v>919</v>
       </c>
@@ -1416,7 +1755,7 @@
       <c r="S5" s="18"/>
       <c r="T5" s="10"/>
     </row>
-    <row r="6" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -1448,10 +1787,18 @@
       <c r="K6" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="14"/>
+      <c r="L6" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="N6" s="13">
+        <v>42436</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>181</v>
+      </c>
       <c r="P6" s="22">
         <v>1220</v>
       </c>
@@ -1462,7 +1809,7 @@
       <c r="S6" s="18"/>
       <c r="T6" s="10"/>
     </row>
-    <row r="7" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -1494,10 +1841,18 @@
       <c r="K7" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="L7" s="12"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="14"/>
+      <c r="L7" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="N7" s="13">
+        <v>42436</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>181</v>
+      </c>
       <c r="P7" s="22">
         <v>1222</v>
       </c>
@@ -1508,7 +1863,7 @@
       <c r="S7" s="18"/>
       <c r="T7" s="10"/>
     </row>
-    <row r="8" spans="1:20" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" s="11" customFormat="1" ht="33" x14ac:dyDescent="0.35">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -1552,7 +1907,7 @@
       <c r="S8" s="18"/>
       <c r="T8" s="10"/>
     </row>
-    <row r="9" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -1596,7 +1951,7 @@
       <c r="S9" s="18"/>
       <c r="T9" s="10"/>
     </row>
-    <row r="10" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A10" s="21">
         <v>9</v>
       </c>
@@ -1640,7 +1995,7 @@
       <c r="S10" s="18"/>
       <c r="T10" s="10"/>
     </row>
-    <row r="11" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -1684,7 +2039,7 @@
       <c r="S11" s="18"/>
       <c r="T11" s="10"/>
     </row>
-    <row r="12" spans="1:20" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" s="11" customFormat="1" ht="33" x14ac:dyDescent="0.35">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -1728,7 +2083,7 @@
       <c r="S12" s="18"/>
       <c r="T12" s="10"/>
     </row>
-    <row r="13" spans="1:20" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" s="11" customFormat="1" ht="33" x14ac:dyDescent="0.35">
       <c r="A13" s="21">
         <v>12</v>
       </c>
@@ -1772,7 +2127,7 @@
       <c r="S13" s="18"/>
       <c r="T13" s="10"/>
     </row>
-    <row r="14" spans="1:20" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A14" s="21">
         <v>13</v>
       </c>
@@ -1816,7 +2171,7 @@
       <c r="S14" s="18"/>
       <c r="T14" s="10"/>
     </row>
-    <row r="15" spans="1:20" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" s="11" customFormat="1" ht="33" x14ac:dyDescent="0.35">
       <c r="A15" s="21">
         <v>14</v>
       </c>
@@ -1860,7 +2215,7 @@
       <c r="S15" s="18"/>
       <c r="T15" s="10"/>
     </row>
-    <row r="16" spans="1:20" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" s="11" customFormat="1" ht="33" x14ac:dyDescent="0.35">
       <c r="A16" s="21">
         <v>15</v>
       </c>
@@ -1904,7 +2259,7 @@
       <c r="S16" s="18"/>
       <c r="T16" s="10"/>
     </row>
-    <row r="17" spans="1:20" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" s="11" customFormat="1" ht="33" x14ac:dyDescent="0.35">
       <c r="A17" s="21">
         <v>16</v>
       </c>
@@ -1948,7 +2303,7 @@
       <c r="S17" s="18"/>
       <c r="T17" s="10"/>
     </row>
-    <row r="18" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A18" s="21">
         <v>17</v>
       </c>
@@ -1990,7 +2345,7 @@
       <c r="S18" s="18"/>
       <c r="T18" s="10"/>
     </row>
-    <row r="19" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A19" s="21">
         <v>18</v>
       </c>
@@ -2034,7 +2389,7 @@
       <c r="S19" s="18"/>
       <c r="T19" s="10"/>
     </row>
-    <row r="20" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A20" s="21">
         <v>19</v>
       </c>
@@ -2078,7 +2433,7 @@
       <c r="S20" s="18"/>
       <c r="T20" s="10"/>
     </row>
-    <row r="21" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A21" s="21">
         <v>20</v>
       </c>
@@ -2120,7 +2475,7 @@
       <c r="S21" s="18"/>
       <c r="T21" s="10"/>
     </row>
-    <row r="22" spans="1:20" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" s="11" customFormat="1" ht="33" x14ac:dyDescent="0.35">
       <c r="A22" s="21">
         <v>21</v>
       </c>
@@ -2162,7 +2517,7 @@
       <c r="S22" s="18"/>
       <c r="T22" s="10"/>
     </row>
-    <row r="23" spans="1:20" s="39" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" s="39" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A23" s="21">
         <v>22</v>
       </c>
@@ -2203,7 +2558,7 @@
       <c r="R23" s="38"/>
       <c r="S23" s="18"/>
     </row>
-    <row r="24" spans="1:20" s="39" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" s="39" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A24" s="21">
         <v>23</v>
       </c>
@@ -2244,7 +2599,7 @@
       <c r="R24" s="38"/>
       <c r="S24" s="18"/>
     </row>
-    <row r="25" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A25" s="21">
         <v>24</v>
       </c>
@@ -2370,7 +2725,7 @@
       <c r="S27" s="18"/>
       <c r="T27" s="10"/>
     </row>
-    <row r="28" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A28" s="21">
         <v>27</v>
       </c>
@@ -2412,381 +2767,858 @@
       <c r="S28" s="18"/>
       <c r="T28" s="10"/>
     </row>
-    <row r="29" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="18"/>
+    <row r="29" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="21">
+        <v>28</v>
+      </c>
+      <c r="B29" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F29" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G29" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H29" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I29" s="41"/>
+      <c r="J29" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="K29" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L29" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="M29" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="N29" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O29" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="P29" s="44"/>
+      <c r="Q29" s="44"/>
+      <c r="R29" s="45"/>
+      <c r="S29" s="46"/>
       <c r="T29" s="10"/>
     </row>
-    <row r="30" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="18"/>
+    <row r="30" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="21">
+        <v>29</v>
+      </c>
+      <c r="B30" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G30" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I30" s="41"/>
+      <c r="J30" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="K30" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L30" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="M30" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="N30" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O30" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="P30" s="44"/>
+      <c r="Q30" s="44"/>
+      <c r="R30" s="45"/>
+      <c r="S30" s="46"/>
       <c r="T30" s="10"/>
     </row>
-    <row r="31" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="18"/>
+    <row r="31" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="21">
+        <v>30</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E31" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G31" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H31" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I31" s="41"/>
+      <c r="J31" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="K31" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L31" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="M31" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="N31" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O31" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="P31" s="44"/>
+      <c r="Q31" s="44"/>
+      <c r="R31" s="45"/>
+      <c r="S31" s="46"/>
       <c r="T31" s="10"/>
     </row>
-    <row r="32" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="14"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="18"/>
+    <row r="32" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="21">
+        <v>31</v>
+      </c>
+      <c r="B32" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E32" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G32" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I32" s="41"/>
+      <c r="J32" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="K32" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L32" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="M32" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="N32" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O32" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="P32" s="44"/>
+      <c r="Q32" s="44"/>
+      <c r="R32" s="45"/>
+      <c r="S32" s="46"/>
       <c r="T32" s="10"/>
     </row>
-    <row r="33" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="18"/>
+    <row r="33" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="21">
+        <v>32</v>
+      </c>
+      <c r="B33" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E33" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G33" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H33" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I33" s="41"/>
+      <c r="J33" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="K33" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L33" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="M33" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="N33" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O33" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="P33" s="44"/>
+      <c r="Q33" s="44"/>
+      <c r="R33" s="45"/>
+      <c r="S33" s="46"/>
       <c r="T33" s="10"/>
     </row>
-    <row r="34" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="7"/>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="7"/>
-      <c r="S34" s="18"/>
+    <row r="34" spans="1:20" s="11" customFormat="1" ht="33" x14ac:dyDescent="0.35">
+      <c r="A34" s="21">
+        <v>33</v>
+      </c>
+      <c r="B34" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E34" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G34" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H34" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I34" s="41"/>
+      <c r="J34" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="K34" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L34" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="M34" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="N34" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O34" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="P34" s="44"/>
+      <c r="Q34" s="44"/>
+      <c r="R34" s="45"/>
+      <c r="S34" s="46"/>
       <c r="T34" s="10"/>
     </row>
-    <row r="35" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="7"/>
-      <c r="Q35" s="7"/>
-      <c r="R35" s="7"/>
-      <c r="S35" s="18"/>
+    <row r="35" spans="1:20" s="11" customFormat="1" ht="33" x14ac:dyDescent="0.35">
+      <c r="A35" s="21">
+        <v>34</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E35" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G35" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H35" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I35" s="41"/>
+      <c r="J35" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="K35" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L35" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="M35" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="N35" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O35" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="P35" s="44"/>
+      <c r="Q35" s="44"/>
+      <c r="R35" s="45"/>
+      <c r="S35" s="46"/>
       <c r="T35" s="10"/>
     </row>
-    <row r="36" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7"/>
-      <c r="R36" s="7"/>
-      <c r="S36" s="18"/>
+    <row r="36" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="21">
+        <v>35</v>
+      </c>
+      <c r="B36" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="E36" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G36" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H36" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I36" s="41"/>
+      <c r="J36" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="K36" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L36" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="M36" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="N36" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O36" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="P36" s="44"/>
+      <c r="Q36" s="44"/>
+      <c r="R36" s="45"/>
+      <c r="S36" s="46"/>
       <c r="T36" s="10"/>
     </row>
-    <row r="37" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="7"/>
-      <c r="R37" s="7"/>
-      <c r="S37" s="18"/>
+    <row r="37" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="21">
+        <v>36</v>
+      </c>
+      <c r="B37" s="40" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="D37" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="E37" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G37" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H37" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I37" s="41"/>
+      <c r="J37" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="K37" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L37" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="M37" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="N37" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O37" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="P37" s="44"/>
+      <c r="Q37" s="44"/>
+      <c r="R37" s="45"/>
+      <c r="S37" s="46" t="s">
+        <v>150</v>
+      </c>
       <c r="T37" s="10"/>
     </row>
-    <row r="38" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="13"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="7"/>
-      <c r="R38" s="7"/>
-      <c r="S38" s="18"/>
+    <row r="38" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="21">
+        <v>37</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C38" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E38" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G38" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H38" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I38" s="41"/>
+      <c r="J38" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="K38" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L38" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="M38" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="N38" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O38" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="P38" s="44"/>
+      <c r="Q38" s="44"/>
+      <c r="R38" s="45"/>
+      <c r="S38" s="46"/>
       <c r="T38" s="10"/>
     </row>
-    <row r="39" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="12"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="13"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="7"/>
-      <c r="R39" s="7"/>
-      <c r="S39" s="18"/>
+    <row r="39" spans="1:20" s="11" customFormat="1" ht="49.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="21">
+        <v>38</v>
+      </c>
+      <c r="B39" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="D39" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="E39" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G39" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H39" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I39" s="41"/>
+      <c r="J39" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="K39" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L39" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="M39" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="N39" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O39" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="P39" s="44"/>
+      <c r="Q39" s="44"/>
+      <c r="R39" s="45"/>
+      <c r="S39" s="47" t="s">
+        <v>157</v>
+      </c>
       <c r="T39" s="10"/>
     </row>
-    <row r="40" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="12"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="14"/>
+    <row r="40" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="21">
+        <v>39</v>
+      </c>
+      <c r="B40" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="E40" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G40" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H40" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I40" s="41"/>
+      <c r="J40" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="K40" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L40" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="M40" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="N40" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O40" s="43" t="s">
+        <v>121</v>
+      </c>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
-      <c r="R40" s="7"/>
-      <c r="S40" s="18"/>
+      <c r="R40" s="45"/>
       <c r="T40" s="10"/>
     </row>
-    <row r="41" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="14"/>
+    <row r="41" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="21">
+        <v>40</v>
+      </c>
+      <c r="B41" s="48" t="s">
+        <v>159</v>
+      </c>
+      <c r="C41" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G41" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H41" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I41" s="41"/>
+      <c r="J41" s="43" t="s">
+        <v>160</v>
+      </c>
+      <c r="K41" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="L41" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="M41" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="N41" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O41" s="43" t="s">
+        <v>162</v>
+      </c>
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
-      <c r="R41" s="7"/>
-      <c r="S41" s="18"/>
+      <c r="R41" s="45"/>
+      <c r="S41" s="46"/>
       <c r="T41" s="10"/>
     </row>
-    <row r="42" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="12"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="14"/>
+    <row r="42" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="21">
+        <v>41</v>
+      </c>
+      <c r="B42" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="C42" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E42" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F42" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G42" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H42" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I42" s="41"/>
+      <c r="J42" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="K42" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L42" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="M42" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="N42" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O42" s="43" t="s">
+        <v>130</v>
+      </c>
       <c r="P42" s="7"/>
       <c r="Q42" s="7"/>
-      <c r="R42" s="7"/>
-      <c r="S42" s="18"/>
+      <c r="R42" s="45"/>
+      <c r="S42" s="46"/>
       <c r="T42" s="10"/>
     </row>
-    <row r="43" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="12"/>
-      <c r="L43" s="12"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="13"/>
-      <c r="O43" s="14"/>
+    <row r="43" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A43" s="21">
+        <v>42</v>
+      </c>
+      <c r="B43" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E43" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G43" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="H43" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I43" s="41"/>
+      <c r="J43" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="K43" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L43" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="M43" s="43" t="s">
+        <v>166</v>
+      </c>
+      <c r="N43" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O43" s="43"/>
       <c r="P43" s="7"/>
       <c r="Q43" s="7"/>
-      <c r="R43" s="7"/>
-      <c r="S43" s="18"/>
+      <c r="R43" s="45"/>
+      <c r="S43" s="46"/>
       <c r="T43" s="10"/>
     </row>
-    <row r="44" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="12"/>
-      <c r="L44" s="12"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="14"/>
+    <row r="44" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A44" s="21">
+        <v>43</v>
+      </c>
+      <c r="B44" s="49" t="s">
+        <v>167</v>
+      </c>
+      <c r="C44" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="D44" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E44" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="F44" s="42">
+        <v>42437</v>
+      </c>
+      <c r="G44" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="H44" s="42">
+        <v>42437</v>
+      </c>
+      <c r="I44" s="41"/>
+      <c r="J44" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="K44" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="L44" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="M44" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="N44" s="42">
+        <v>42437</v>
+      </c>
+      <c r="O44" s="43" t="s">
+        <v>130</v>
+      </c>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
-      <c r="R44" s="7"/>
-      <c r="S44" s="18"/>
+      <c r="R44" s="45"/>
+      <c r="S44" s="46"/>
       <c r="T44" s="10"/>
     </row>
-    <row r="45" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="21"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="13"/>
-      <c r="O45" s="14"/>
+    <row r="45" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A45" s="21">
+        <v>44</v>
+      </c>
+      <c r="B45" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="C45" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D45" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="E45" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="F45" s="42">
+        <v>42438</v>
+      </c>
+      <c r="G45" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="H45" s="42">
+        <v>42438</v>
+      </c>
+      <c r="I45" s="41"/>
+      <c r="J45" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="K45" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="L45" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="M45" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="N45" s="42">
+        <v>42438</v>
+      </c>
+      <c r="O45" s="43" t="s">
+        <v>130</v>
+      </c>
       <c r="P45" s="7"/>
       <c r="Q45" s="7"/>
-      <c r="R45" s="7"/>
-      <c r="S45" s="18"/>
+      <c r="R45" s="45"/>
+      <c r="S45" s="46"/>
       <c r="T45" s="10"/>
     </row>
-    <row r="46" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A46" s="21"/>
       <c r="B46" s="8"/>
       <c r="C46" s="12"/>
@@ -2808,7 +3640,7 @@
       <c r="S46" s="18"/>
       <c r="T46" s="10"/>
     </row>
-    <row r="47" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A47" s="21"/>
       <c r="B47" s="8"/>
       <c r="C47" s="12"/>
@@ -2830,7 +3662,7 @@
       <c r="S47" s="18"/>
       <c r="T47" s="10"/>
     </row>
-    <row r="48" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A48" s="21"/>
       <c r="B48" s="8"/>
       <c r="C48" s="12"/>
@@ -2852,7 +3684,7 @@
       <c r="S48" s="18"/>
       <c r="T48" s="10"/>
     </row>
-    <row r="49" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A49" s="21"/>
       <c r="B49" s="8"/>
       <c r="C49" s="12"/>
@@ -2874,7 +3706,7 @@
       <c r="S49" s="18"/>
       <c r="T49" s="10"/>
     </row>
-    <row r="50" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A50" s="21"/>
       <c r="B50" s="8"/>
       <c r="C50" s="12"/>
@@ -2896,7 +3728,7 @@
       <c r="S50" s="18"/>
       <c r="T50" s="10"/>
     </row>
-    <row r="51" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A51" s="21"/>
       <c r="B51" s="8"/>
       <c r="C51" s="12"/>
@@ -2918,7 +3750,7 @@
       <c r="S51" s="18"/>
       <c r="T51" s="10"/>
     </row>
-    <row r="52" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A52" s="21"/>
       <c r="B52" s="8"/>
       <c r="C52" s="12"/>
@@ -2940,7 +3772,7 @@
       <c r="S52" s="18"/>
       <c r="T52" s="10"/>
     </row>
-    <row r="53" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A53" s="21"/>
       <c r="B53" s="8"/>
       <c r="C53" s="12"/>
@@ -2962,7 +3794,7 @@
       <c r="S53" s="18"/>
       <c r="T53" s="10"/>
     </row>
-    <row r="54" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A54" s="21"/>
       <c r="B54" s="8"/>
       <c r="C54" s="12"/>
@@ -2984,7 +3816,7 @@
       <c r="S54" s="18"/>
       <c r="T54" s="10"/>
     </row>
-    <row r="55" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A55" s="21"/>
       <c r="B55" s="8"/>
       <c r="C55" s="12"/>
@@ -3006,7 +3838,7 @@
       <c r="S55" s="18"/>
       <c r="T55" s="10"/>
     </row>
-    <row r="56" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A56" s="21"/>
       <c r="B56" s="8"/>
       <c r="C56" s="12"/>
@@ -3028,7 +3860,7 @@
       <c r="S56" s="18"/>
       <c r="T56" s="10"/>
     </row>
-    <row r="57" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A57" s="21"/>
       <c r="B57" s="8"/>
       <c r="C57" s="12"/>
@@ -3050,7 +3882,7 @@
       <c r="S57" s="18"/>
       <c r="T57" s="10"/>
     </row>
-    <row r="58" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A58" s="21"/>
       <c r="B58" s="8"/>
       <c r="C58" s="12"/>
@@ -3072,7 +3904,7 @@
       <c r="S58" s="18"/>
       <c r="T58" s="10"/>
     </row>
-    <row r="59" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A59" s="21"/>
       <c r="B59" s="8"/>
       <c r="C59" s="12"/>
@@ -3094,7 +3926,7 @@
       <c r="S59" s="18"/>
       <c r="T59" s="10"/>
     </row>
-    <row r="60" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A60" s="21"/>
       <c r="B60" s="8"/>
       <c r="C60" s="12"/>
@@ -3116,7 +3948,7 @@
       <c r="S60" s="18"/>
       <c r="T60" s="10"/>
     </row>
-    <row r="61" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A61" s="9"/>
       <c r="B61" s="17"/>
       <c r="C61" s="9"/>
@@ -3138,7 +3970,7 @@
       <c r="S61" s="17"/>
       <c r="T61" s="10"/>
     </row>
-    <row r="62" spans="1:20" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" s="11" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A62" s="9"/>
       <c r="B62" s="17"/>
       <c r="C62" s="9"/>
@@ -3160,7 +3992,7 @@
       <c r="S62" s="17"/>
       <c r="T62" s="10"/>
     </row>
-    <row r="63" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A63" s="7"/>
       <c r="B63" s="4"/>
       <c r="C63" s="7"/>
@@ -3181,7 +4013,7 @@
       <c r="R63" s="7"/>
       <c r="S63" s="4"/>
     </row>
-    <row r="64" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A64" s="7"/>
       <c r="B64" s="4"/>
       <c r="C64" s="7"/>
@@ -3202,7 +4034,7 @@
       <c r="R64" s="7"/>
       <c r="S64" s="4"/>
     </row>
-    <row r="65" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A65" s="7"/>
       <c r="B65" s="4"/>
       <c r="C65" s="7"/>
@@ -3223,7 +4055,7 @@
       <c r="R65" s="7"/>
       <c r="S65" s="4"/>
     </row>
-    <row r="66" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A66" s="7"/>
       <c r="B66" s="4"/>
       <c r="C66" s="7"/>
@@ -3244,7 +4076,7 @@
       <c r="R66" s="7"/>
       <c r="S66" s="4"/>
     </row>
-    <row r="67" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A67" s="7"/>
       <c r="B67" s="4"/>
       <c r="C67" s="7"/>
@@ -3265,7 +4097,7 @@
       <c r="R67" s="7"/>
       <c r="S67" s="4"/>
     </row>
-    <row r="68" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A68" s="7"/>
       <c r="B68" s="4"/>
       <c r="C68" s="7"/>
@@ -3286,7 +4118,7 @@
       <c r="R68" s="7"/>
       <c r="S68" s="4"/>
     </row>
-    <row r="69" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A69" s="7"/>
       <c r="B69" s="4"/>
       <c r="C69" s="7"/>
@@ -3307,7 +4139,7 @@
       <c r="R69" s="7"/>
       <c r="S69" s="4"/>
     </row>
-    <row r="70" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A70" s="7"/>
       <c r="B70" s="4"/>
       <c r="C70" s="7"/>
@@ -3328,7 +4160,7 @@
       <c r="R70" s="7"/>
       <c r="S70" s="4"/>
     </row>
-    <row r="71" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A71" s="7"/>
       <c r="B71" s="4"/>
       <c r="C71" s="7"/>
@@ -3349,7 +4181,7 @@
       <c r="R71" s="7"/>
       <c r="S71" s="4"/>
     </row>
-    <row r="72" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A72" s="7"/>
       <c r="B72" s="4"/>
       <c r="C72" s="7"/>
@@ -3370,7 +4202,7 @@
       <c r="R72" s="7"/>
       <c r="S72" s="4"/>
     </row>
-    <row r="73" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A73" s="7"/>
       <c r="B73" s="4"/>
       <c r="C73" s="7"/>
@@ -3391,7 +4223,7 @@
       <c r="R73" s="7"/>
       <c r="S73" s="4"/>
     </row>
-    <row r="74" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A74" s="7"/>
       <c r="B74" s="4"/>
       <c r="C74" s="7"/>
@@ -3412,7 +4244,7 @@
       <c r="R74" s="7"/>
       <c r="S74" s="4"/>
     </row>
-    <row r="75" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A75" s="7"/>
       <c r="B75" s="4"/>
       <c r="C75" s="7"/>
@@ -3433,7 +4265,7 @@
       <c r="R75" s="7"/>
       <c r="S75" s="4"/>
     </row>
-    <row r="76" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A76" s="7"/>
       <c r="B76" s="4"/>
       <c r="C76" s="7"/>
@@ -3454,7 +4286,7 @@
       <c r="R76" s="7"/>
       <c r="S76" s="4"/>
     </row>
-    <row r="77" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A77" s="7"/>
       <c r="B77" s="4"/>
       <c r="C77" s="7"/>
@@ -3475,7 +4307,7 @@
       <c r="R77" s="7"/>
       <c r="S77" s="4"/>
     </row>
-    <row r="78" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A78" s="7"/>
       <c r="B78" s="4"/>
       <c r="C78" s="7"/>
@@ -3496,7 +4328,7 @@
       <c r="R78" s="7"/>
       <c r="S78" s="4"/>
     </row>
-    <row r="79" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A79" s="7"/>
       <c r="B79" s="4"/>
       <c r="C79" s="7"/>
@@ -3517,7 +4349,7 @@
       <c r="R79" s="7"/>
       <c r="S79" s="4"/>
     </row>
-    <row r="80" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A80" s="7"/>
       <c r="B80" s="4"/>
       <c r="C80" s="7"/>
@@ -3538,7 +4370,7 @@
       <c r="R80" s="7"/>
       <c r="S80" s="4"/>
     </row>
-    <row r="81" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A81" s="7"/>
       <c r="B81" s="4"/>
       <c r="C81" s="7"/>
@@ -3559,7 +4391,7 @@
       <c r="R81" s="7"/>
       <c r="S81" s="4"/>
     </row>
-    <row r="82" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A82" s="7"/>
       <c r="B82" s="4"/>
       <c r="C82" s="7"/>
@@ -3580,7 +4412,7 @@
       <c r="R82" s="7"/>
       <c r="S82" s="4"/>
     </row>
-    <row r="83" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A83" s="7"/>
       <c r="B83" s="4"/>
       <c r="C83" s="7"/>
@@ -3601,7 +4433,7 @@
       <c r="R83" s="7"/>
       <c r="S83" s="4"/>
     </row>
-    <row r="84" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A84" s="7"/>
       <c r="B84" s="4"/>
       <c r="C84" s="7"/>
@@ -3622,7 +4454,7 @@
       <c r="R84" s="7"/>
       <c r="S84" s="4"/>
     </row>
-    <row r="85" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A85" s="7"/>
       <c r="B85" s="4"/>
       <c r="C85" s="7"/>
@@ -3643,7 +4475,7 @@
       <c r="R85" s="7"/>
       <c r="S85" s="4"/>
     </row>
-    <row r="86" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A86" s="7"/>
       <c r="B86" s="4"/>
       <c r="C86" s="7"/>
@@ -3664,7 +4496,7 @@
       <c r="R86" s="7"/>
       <c r="S86" s="4"/>
     </row>
-    <row r="87" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A87" s="7"/>
       <c r="B87" s="4"/>
       <c r="C87" s="7"/>
@@ -3685,7 +4517,7 @@
       <c r="R87" s="7"/>
       <c r="S87" s="4"/>
     </row>
-    <row r="88" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A88" s="7"/>
       <c r="B88" s="4"/>
       <c r="C88" s="7"/>
@@ -3706,7 +4538,7 @@
       <c r="R88" s="7"/>
       <c r="S88" s="4"/>
     </row>
-    <row r="89" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A89" s="7"/>
       <c r="B89" s="4"/>
       <c r="C89" s="7"/>
@@ -3727,7 +4559,7 @@
       <c r="R89" s="7"/>
       <c r="S89" s="4"/>
     </row>
-    <row r="90" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A90" s="7"/>
       <c r="B90" s="4"/>
       <c r="C90" s="7"/>
@@ -3748,7 +4580,7 @@
       <c r="R90" s="7"/>
       <c r="S90" s="4"/>
     </row>
-    <row r="91" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A91" s="7"/>
       <c r="B91" s="4"/>
       <c r="C91" s="7"/>
@@ -3769,7 +4601,7 @@
       <c r="R91" s="7"/>
       <c r="S91" s="4"/>
     </row>
-    <row r="92" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A92" s="7"/>
       <c r="B92" s="4"/>
       <c r="C92" s="7"/>
@@ -3790,7 +4622,7 @@
       <c r="R92" s="7"/>
       <c r="S92" s="4"/>
     </row>
-    <row r="93" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A93" s="7"/>
       <c r="B93" s="4"/>
       <c r="C93" s="7"/>
@@ -3811,7 +4643,7 @@
       <c r="R93" s="7"/>
       <c r="S93" s="4"/>
     </row>
-    <row r="94" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A94" s="7"/>
       <c r="B94" s="4"/>
       <c r="C94" s="7"/>
@@ -3832,7 +4664,7 @@
       <c r="R94" s="7"/>
       <c r="S94" s="4"/>
     </row>
-    <row r="95" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A95" s="7"/>
       <c r="B95" s="4"/>
       <c r="C95" s="7"/>
@@ -3853,7 +4685,7 @@
       <c r="R95" s="7"/>
       <c r="S95" s="4"/>
     </row>
-    <row r="96" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A96" s="7"/>
       <c r="B96" s="4"/>
       <c r="C96" s="7"/>
@@ -3874,7 +4706,7 @@
       <c r="R96" s="7"/>
       <c r="S96" s="4"/>
     </row>
-    <row r="97" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A97" s="7"/>
       <c r="B97" s="4"/>
       <c r="C97" s="7"/>
@@ -3895,7 +4727,7 @@
       <c r="R97" s="7"/>
       <c r="S97" s="4"/>
     </row>
-    <row r="98" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A98" s="7"/>
       <c r="B98" s="4"/>
       <c r="C98" s="7"/>
@@ -3916,7 +4748,7 @@
       <c r="R98" s="7"/>
       <c r="S98" s="4"/>
     </row>
-    <row r="99" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A99" s="7"/>
       <c r="B99" s="4"/>
       <c r="C99" s="7"/>
@@ -3937,7 +4769,7 @@
       <c r="R99" s="7"/>
       <c r="S99" s="4"/>
     </row>
-    <row r="100" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A100" s="7"/>
       <c r="B100" s="4"/>
       <c r="C100" s="7"/>
@@ -3958,7 +4790,7 @@
       <c r="R100" s="7"/>
       <c r="S100" s="4"/>
     </row>
-    <row r="101" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A101" s="7"/>
       <c r="B101" s="4"/>
       <c r="C101" s="7"/>
@@ -3979,7 +4811,7 @@
       <c r="R101" s="7"/>
       <c r="S101" s="4"/>
     </row>
-    <row r="102" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A102" s="7"/>
       <c r="B102" s="4"/>
       <c r="C102" s="7"/>
@@ -4000,7 +4832,7 @@
       <c r="R102" s="7"/>
       <c r="S102" s="4"/>
     </row>
-    <row r="103" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A103" s="7"/>
       <c r="B103" s="4"/>
       <c r="C103" s="7"/>
@@ -4021,7 +4853,7 @@
       <c r="R103" s="7"/>
       <c r="S103" s="4"/>
     </row>
-    <row r="104" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A104" s="7"/>
       <c r="B104" s="4"/>
       <c r="C104" s="7"/>
@@ -4042,7 +4874,7 @@
       <c r="R104" s="7"/>
       <c r="S104" s="4"/>
     </row>
-    <row r="105" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A105" s="7"/>
       <c r="B105" s="4"/>
       <c r="C105" s="7"/>
@@ -4063,7 +4895,7 @@
       <c r="R105" s="7"/>
       <c r="S105" s="4"/>
     </row>
-    <row r="106" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A106" s="7"/>
       <c r="B106" s="4"/>
       <c r="C106" s="7"/>
@@ -4084,7 +4916,7 @@
       <c r="R106" s="7"/>
       <c r="S106" s="4"/>
     </row>
-    <row r="107" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A107" s="7"/>
       <c r="B107" s="4"/>
       <c r="C107" s="7"/>
@@ -4105,7 +4937,7 @@
       <c r="R107" s="7"/>
       <c r="S107" s="4"/>
     </row>
-    <row r="108" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A108" s="7"/>
       <c r="B108" s="4"/>
       <c r="C108" s="7"/>
@@ -4126,7 +4958,7 @@
       <c r="R108" s="7"/>
       <c r="S108" s="4"/>
     </row>
-    <row r="109" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A109" s="7"/>
       <c r="B109" s="4"/>
       <c r="C109" s="7"/>
@@ -4147,7 +4979,7 @@
       <c r="R109" s="7"/>
       <c r="S109" s="4"/>
     </row>
-    <row r="110" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A110" s="7"/>
       <c r="B110" s="4"/>
       <c r="C110" s="7"/>
@@ -4168,7 +5000,7 @@
       <c r="R110" s="7"/>
       <c r="S110" s="4"/>
     </row>
-    <row r="111" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A111" s="7"/>
       <c r="B111" s="4"/>
       <c r="C111" s="7"/>
@@ -4189,7 +5021,7 @@
       <c r="R111" s="7"/>
       <c r="S111" s="4"/>
     </row>
-    <row r="112" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A112" s="7"/>
       <c r="B112" s="4"/>
       <c r="C112" s="7"/>
@@ -4210,7 +5042,7 @@
       <c r="R112" s="7"/>
       <c r="S112" s="4"/>
     </row>
-    <row r="113" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A113" s="7"/>
       <c r="B113" s="4"/>
       <c r="C113" s="7"/>
@@ -4231,7 +5063,7 @@
       <c r="R113" s="7"/>
       <c r="S113" s="4"/>
     </row>
-    <row r="114" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A114" s="7"/>
       <c r="B114" s="4"/>
       <c r="C114" s="7"/>
@@ -4252,7 +5084,7 @@
       <c r="R114" s="7"/>
       <c r="S114" s="4"/>
     </row>
-    <row r="115" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A115" s="7"/>
       <c r="B115" s="4"/>
       <c r="C115" s="7"/>
@@ -4273,7 +5105,7 @@
       <c r="R115" s="7"/>
       <c r="S115" s="4"/>
     </row>
-    <row r="116" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A116" s="7"/>
       <c r="B116" s="4"/>
       <c r="C116" s="7"/>
@@ -4294,7 +5126,7 @@
       <c r="R116" s="7"/>
       <c r="S116" s="4"/>
     </row>
-    <row r="117" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A117" s="7"/>
       <c r="B117" s="4"/>
       <c r="C117" s="7"/>
@@ -4315,7 +5147,7 @@
       <c r="R117" s="7"/>
       <c r="S117" s="4"/>
     </row>
-    <row r="118" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A118" s="7"/>
       <c r="B118" s="4"/>
       <c r="C118" s="7"/>
@@ -4336,7 +5168,7 @@
       <c r="R118" s="7"/>
       <c r="S118" s="4"/>
     </row>
-    <row r="119" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A119" s="7"/>
       <c r="B119" s="4"/>
       <c r="C119" s="7"/>
@@ -4357,7 +5189,7 @@
       <c r="R119" s="7"/>
       <c r="S119" s="4"/>
     </row>
-    <row r="120" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A120" s="7"/>
       <c r="B120" s="4"/>
       <c r="C120" s="7"/>
@@ -4378,7 +5210,7 @@
       <c r="R120" s="7"/>
       <c r="S120" s="4"/>
     </row>
-    <row r="121" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A121" s="7"/>
       <c r="B121" s="4"/>
       <c r="C121" s="7"/>
@@ -4399,7 +5231,7 @@
       <c r="R121" s="7"/>
       <c r="S121" s="4"/>
     </row>
-    <row r="122" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A122" s="7"/>
       <c r="B122" s="4"/>
       <c r="C122" s="7"/>
@@ -4420,7 +5252,7 @@
       <c r="R122" s="7"/>
       <c r="S122" s="4"/>
     </row>
-    <row r="123" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" ht="16.5" x14ac:dyDescent="0.15">
       <c r="A123" s="7"/>
       <c r="B123" s="4"/>
       <c r="C123" s="7"/>
@@ -4441,7 +5273,7 @@
       <c r="R123" s="7"/>
       <c r="S123" s="4"/>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A124" s="7"/>
       <c r="B124" s="4"/>
       <c r="C124" s="7"/>
@@ -4462,7 +5294,7 @@
       <c r="R124" s="7"/>
       <c r="S124" s="4"/>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A125" s="7"/>
       <c r="B125" s="4"/>
       <c r="C125" s="7"/>
@@ -4483,7 +5315,7 @@
       <c r="R125" s="7"/>
       <c r="S125" s="4"/>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A126" s="7"/>
       <c r="B126" s="4"/>
       <c r="C126" s="7"/>
@@ -4504,7 +5336,7 @@
       <c r="R126" s="7"/>
       <c r="S126" s="4"/>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A127" s="7"/>
       <c r="B127" s="4"/>
       <c r="C127" s="7"/>
@@ -4525,7 +5357,7 @@
       <c r="R127" s="7"/>
       <c r="S127" s="4"/>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A128" s="7"/>
       <c r="B128" s="4"/>
       <c r="C128" s="7"/>
@@ -4546,7 +5378,7 @@
       <c r="R128" s="7"/>
       <c r="S128" s="4"/>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A129" s="7"/>
       <c r="B129" s="4"/>
       <c r="C129" s="7"/>
@@ -4567,7 +5399,7 @@
       <c r="R129" s="7"/>
       <c r="S129" s="4"/>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A130" s="7"/>
       <c r="B130" s="4"/>
       <c r="C130" s="7"/>
@@ -4588,7 +5420,7 @@
       <c r="R130" s="7"/>
       <c r="S130" s="4"/>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A131" s="7"/>
       <c r="B131" s="4"/>
       <c r="C131" s="7"/>
@@ -4609,7 +5441,7 @@
       <c r="R131" s="7"/>
       <c r="S131" s="4"/>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A132" s="7"/>
       <c r="B132" s="4"/>
       <c r="C132" s="7"/>
@@ -4630,7 +5462,7 @@
       <c r="R132" s="7"/>
       <c r="S132" s="4"/>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A133" s="7"/>
       <c r="B133" s="4"/>
       <c r="C133" s="7"/>
@@ -4651,7 +5483,7 @@
       <c r="R133" s="7"/>
       <c r="S133" s="4"/>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A134" s="7"/>
       <c r="B134" s="4"/>
       <c r="C134" s="7"/>
@@ -4672,7 +5504,7 @@
       <c r="R134" s="7"/>
       <c r="S134" s="4"/>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A135" s="7"/>
       <c r="B135" s="4"/>
       <c r="C135" s="7"/>
@@ -4693,7 +5525,7 @@
       <c r="R135" s="7"/>
       <c r="S135" s="4"/>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A136" s="7"/>
       <c r="B136" s="4"/>
       <c r="C136" s="7"/>
@@ -4714,7 +5546,7 @@
       <c r="R136" s="7"/>
       <c r="S136" s="4"/>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A137" s="7"/>
       <c r="B137" s="4"/>
       <c r="C137" s="7"/>
@@ -4735,7 +5567,7 @@
       <c r="R137" s="7"/>
       <c r="S137" s="4"/>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A138" s="7"/>
       <c r="B138" s="4"/>
       <c r="C138" s="7"/>
@@ -4756,7 +5588,7 @@
       <c r="R138" s="7"/>
       <c r="S138" s="4"/>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A139" s="7"/>
       <c r="B139" s="4"/>
       <c r="C139" s="7"/>
@@ -4777,7 +5609,7 @@
       <c r="R139" s="7"/>
       <c r="S139" s="4"/>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A140" s="7"/>
       <c r="B140" s="4"/>
       <c r="C140" s="7"/>
@@ -4798,7 +5630,7 @@
       <c r="R140" s="7"/>
       <c r="S140" s="4"/>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A141" s="7"/>
       <c r="B141" s="4"/>
       <c r="C141" s="7"/>
@@ -4819,7 +5651,7 @@
       <c r="R141" s="7"/>
       <c r="S141" s="4"/>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A142" s="7"/>
       <c r="B142" s="4"/>
       <c r="C142" s="7"/>
@@ -4840,7 +5672,7 @@
       <c r="R142" s="7"/>
       <c r="S142" s="4"/>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A143" s="7"/>
       <c r="B143" s="4"/>
       <c r="C143" s="7"/>
@@ -4861,7 +5693,7 @@
       <c r="R143" s="7"/>
       <c r="S143" s="4"/>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A144" s="7"/>
       <c r="B144" s="4"/>
       <c r="C144" s="7"/>
@@ -4882,7 +5714,7 @@
       <c r="R144" s="7"/>
       <c r="S144" s="4"/>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A145" s="7"/>
       <c r="B145" s="4"/>
       <c r="C145" s="7"/>
@@ -4903,7 +5735,7 @@
       <c r="R145" s="7"/>
       <c r="S145" s="4"/>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A146" s="7"/>
       <c r="B146" s="4"/>
       <c r="C146" s="7"/>
@@ -4924,7 +5756,7 @@
       <c r="R146" s="7"/>
       <c r="S146" s="4"/>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A147" s="7"/>
       <c r="B147" s="4"/>
       <c r="C147" s="7"/>
@@ -4945,7 +5777,7 @@
       <c r="R147" s="7"/>
       <c r="S147" s="4"/>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A148" s="7"/>
       <c r="B148" s="4"/>
       <c r="C148" s="7"/>
@@ -4966,7 +5798,7 @@
       <c r="R148" s="7"/>
       <c r="S148" s="4"/>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A149" s="7"/>
       <c r="B149" s="4"/>
       <c r="C149" s="7"/>
@@ -4987,7 +5819,7 @@
       <c r="R149" s="7"/>
       <c r="S149" s="4"/>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A150" s="7"/>
       <c r="B150" s="4"/>
       <c r="C150" s="7"/>
@@ -5008,7 +5840,7 @@
       <c r="R150" s="7"/>
       <c r="S150" s="4"/>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A151" s="7"/>
       <c r="B151" s="4"/>
       <c r="C151" s="7"/>
@@ -5029,7 +5861,7 @@
       <c r="R151" s="7"/>
       <c r="S151" s="4"/>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A152" s="7"/>
       <c r="B152" s="4"/>
       <c r="C152" s="7"/>
@@ -5050,7 +5882,7 @@
       <c r="R152" s="7"/>
       <c r="S152" s="4"/>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A153" s="7"/>
       <c r="B153" s="4"/>
       <c r="C153" s="7"/>
@@ -5071,7 +5903,7 @@
       <c r="R153" s="7"/>
       <c r="S153" s="4"/>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A154" s="7"/>
       <c r="B154" s="4"/>
       <c r="C154" s="7"/>
@@ -5092,7 +5924,7 @@
       <c r="R154" s="7"/>
       <c r="S154" s="4"/>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A155" s="7"/>
       <c r="B155" s="4"/>
       <c r="C155" s="7"/>
@@ -5113,7 +5945,7 @@
       <c r="R155" s="7"/>
       <c r="S155" s="4"/>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A156" s="7"/>
       <c r="B156" s="4"/>
       <c r="C156" s="7"/>
@@ -5134,7 +5966,7 @@
       <c r="R156" s="7"/>
       <c r="S156" s="4"/>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A157" s="7"/>
       <c r="B157" s="4"/>
       <c r="C157" s="7"/>
@@ -5155,7 +5987,7 @@
       <c r="R157" s="7"/>
       <c r="S157" s="4"/>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A158" s="7"/>
       <c r="B158" s="4"/>
       <c r="C158" s="7"/>
@@ -5176,7 +6008,7 @@
       <c r="R158" s="7"/>
       <c r="S158" s="4"/>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A159" s="7"/>
       <c r="B159" s="4"/>
       <c r="C159" s="7"/>
@@ -5197,7 +6029,7 @@
       <c r="R159" s="7"/>
       <c r="S159" s="4"/>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A160" s="7"/>
       <c r="B160" s="4"/>
       <c r="C160" s="7"/>
@@ -5218,7 +6050,7 @@
       <c r="R160" s="7"/>
       <c r="S160" s="4"/>
     </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A161" s="7"/>
       <c r="B161" s="4"/>
       <c r="C161" s="7"/>
@@ -5239,7 +6071,7 @@
       <c r="R161" s="7"/>
       <c r="S161" s="4"/>
     </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A162" s="7"/>
       <c r="B162" s="4"/>
       <c r="C162" s="7"/>
@@ -5260,7 +6092,7 @@
       <c r="R162" s="7"/>
       <c r="S162" s="4"/>
     </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A163" s="7"/>
       <c r="B163" s="4"/>
       <c r="C163" s="7"/>
@@ -5281,7 +6113,7 @@
       <c r="R163" s="7"/>
       <c r="S163" s="4"/>
     </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A164" s="7"/>
       <c r="B164" s="4"/>
       <c r="C164" s="7"/>
@@ -5302,7 +6134,7 @@
       <c r="R164" s="7"/>
       <c r="S164" s="4"/>
     </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A165" s="7"/>
       <c r="B165" s="4"/>
       <c r="C165" s="7"/>
@@ -5323,7 +6155,7 @@
       <c r="R165" s="7"/>
       <c r="S165" s="4"/>
     </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A166" s="7"/>
       <c r="B166" s="4"/>
       <c r="C166" s="7"/>
@@ -5344,7 +6176,7 @@
       <c r="R166" s="7"/>
       <c r="S166" s="4"/>
     </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A167" s="7"/>
       <c r="B167" s="4"/>
       <c r="C167" s="7"/>
@@ -5365,7 +6197,7 @@
       <c r="R167" s="7"/>
       <c r="S167" s="4"/>
     </row>
-    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A168" s="7"/>
       <c r="B168" s="4"/>
       <c r="C168" s="7"/>
@@ -5386,7 +6218,7 @@
       <c r="R168" s="7"/>
       <c r="S168" s="4"/>
     </row>
-    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A169" s="7"/>
       <c r="B169" s="4"/>
       <c r="C169" s="7"/>
@@ -5407,7 +6239,7 @@
       <c r="R169" s="7"/>
       <c r="S169" s="4"/>
     </row>
-    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A170" s="7"/>
       <c r="B170" s="4"/>
       <c r="C170" s="7"/>
@@ -5428,7 +6260,7 @@
       <c r="R170" s="7"/>
       <c r="S170" s="4"/>
     </row>
-    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A171" s="7"/>
       <c r="B171" s="4"/>
       <c r="C171" s="7"/>
@@ -5449,7 +6281,7 @@
       <c r="R171" s="7"/>
       <c r="S171" s="4"/>
     </row>
-    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A172" s="7"/>
       <c r="B172" s="4"/>
       <c r="C172" s="7"/>
@@ -5470,7 +6302,7 @@
       <c r="R172" s="7"/>
       <c r="S172" s="4"/>
     </row>
-    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A173" s="7"/>
       <c r="B173" s="4"/>
       <c r="C173" s="7"/>
@@ -5491,7 +6323,7 @@
       <c r="R173" s="7"/>
       <c r="S173" s="4"/>
     </row>
-    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A174" s="7"/>
       <c r="B174" s="4"/>
       <c r="C174" s="7"/>
@@ -5512,7 +6344,7 @@
       <c r="R174" s="7"/>
       <c r="S174" s="4"/>
     </row>
-    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A175" s="7"/>
       <c r="B175" s="4"/>
       <c r="C175" s="7"/>
@@ -5533,7 +6365,7 @@
       <c r="R175" s="7"/>
       <c r="S175" s="4"/>
     </row>
-    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A176" s="7"/>
       <c r="B176" s="4"/>
       <c r="C176" s="7"/>
@@ -5554,7 +6386,7 @@
       <c r="R176" s="7"/>
       <c r="S176" s="4"/>
     </row>
-    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A177" s="7"/>
       <c r="B177" s="4"/>
       <c r="C177" s="7"/>
@@ -5575,7 +6407,7 @@
       <c r="R177" s="7"/>
       <c r="S177" s="4"/>
     </row>
-    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A178" s="7"/>
       <c r="B178" s="4"/>
       <c r="C178" s="7"/>
@@ -5596,7 +6428,7 @@
       <c r="R178" s="7"/>
       <c r="S178" s="4"/>
     </row>
-    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A179" s="7"/>
       <c r="B179" s="4"/>
       <c r="C179" s="7"/>
@@ -5617,7 +6449,7 @@
       <c r="R179" s="7"/>
       <c r="S179" s="4"/>
     </row>
-    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A180" s="7"/>
       <c r="B180" s="4"/>
       <c r="C180" s="7"/>
@@ -5638,7 +6470,7 @@
       <c r="R180" s="7"/>
       <c r="S180" s="4"/>
     </row>
-    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A181" s="7"/>
       <c r="B181" s="4"/>
       <c r="C181" s="7"/>
@@ -5659,7 +6491,7 @@
       <c r="R181" s="7"/>
       <c r="S181" s="4"/>
     </row>
-    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A182" s="7"/>
       <c r="B182" s="4"/>
       <c r="C182" s="7"/>
@@ -5680,7 +6512,7 @@
       <c r="R182" s="7"/>
       <c r="S182" s="4"/>
     </row>
-    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A183" s="7"/>
       <c r="B183" s="4"/>
       <c r="C183" s="7"/>
@@ -5701,7 +6533,7 @@
       <c r="R183" s="7"/>
       <c r="S183" s="4"/>
     </row>
-    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A184" s="7"/>
       <c r="B184" s="4"/>
       <c r="C184" s="7"/>
@@ -5719,7 +6551,7 @@
       <c r="O184" s="4"/>
       <c r="S184" s="4"/>
     </row>
-    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A185" s="7"/>
       <c r="B185" s="4"/>
       <c r="C185" s="7"/>
@@ -5737,7 +6569,7 @@
       <c r="O185" s="4"/>
       <c r="S185" s="4"/>
     </row>
-    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A186" s="7"/>
       <c r="B186" s="4"/>
       <c r="C186" s="7"/>
@@ -5755,7 +6587,7 @@
       <c r="O186" s="4"/>
       <c r="S186" s="4"/>
     </row>
-    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A187" s="7"/>
       <c r="B187" s="4"/>
       <c r="C187" s="7"/>
@@ -5773,7 +6605,7 @@
       <c r="O187" s="4"/>
       <c r="S187" s="4"/>
     </row>
-    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A188" s="7"/>
       <c r="B188" s="4"/>
       <c r="C188" s="7"/>
@@ -5791,7 +6623,7 @@
       <c r="O188" s="4"/>
       <c r="S188" s="4"/>
     </row>
-    <row r="189" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A189" s="7"/>
       <c r="B189" s="4"/>
       <c r="C189" s="7"/>
@@ -5809,7 +6641,7 @@
       <c r="O189" s="4"/>
       <c r="S189" s="4"/>
     </row>
-    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A190" s="7"/>
       <c r="B190" s="4"/>
       <c r="C190" s="7"/>
@@ -5827,7 +6659,7 @@
       <c r="O190" s="4"/>
       <c r="S190" s="4"/>
     </row>
-    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A191" s="7"/>
       <c r="B191" s="4"/>
       <c r="C191" s="7"/>
@@ -5845,7 +6677,7 @@
       <c r="O191" s="4"/>
       <c r="S191" s="4"/>
     </row>
-    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A192" s="7"/>
       <c r="B192" s="4"/>
       <c r="C192" s="7"/>
@@ -5863,7 +6695,7 @@
       <c r="O192" s="4"/>
       <c r="S192" s="4"/>
     </row>
-    <row r="193" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A193" s="7"/>
       <c r="B193" s="4"/>
       <c r="C193" s="7"/>
@@ -5881,7 +6713,7 @@
       <c r="O193" s="4"/>
       <c r="S193" s="4"/>
     </row>
-    <row r="194" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A194" s="7"/>
       <c r="B194" s="4"/>
       <c r="C194" s="7"/>
@@ -5899,7 +6731,7 @@
       <c r="O194" s="4"/>
       <c r="S194" s="4"/>
     </row>
-    <row r="195" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A195" s="7"/>
       <c r="B195" s="4"/>
       <c r="C195" s="7"/>
@@ -5917,7 +6749,7 @@
       <c r="O195" s="4"/>
       <c r="S195" s="4"/>
     </row>
-    <row r="196" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A196" s="7"/>
       <c r="B196" s="4"/>
       <c r="C196" s="7"/>
@@ -5935,7 +6767,7 @@
       <c r="O196" s="4"/>
       <c r="S196" s="4"/>
     </row>
-    <row r="197" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A197" s="7"/>
       <c r="B197" s="4"/>
       <c r="C197" s="7"/>
@@ -5953,7 +6785,7 @@
       <c r="O197" s="4"/>
       <c r="S197" s="4"/>
     </row>
-    <row r="198" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A198" s="7"/>
       <c r="B198" s="4"/>
       <c r="C198" s="7"/>
@@ -5971,7 +6803,7 @@
       <c r="O198" s="4"/>
       <c r="S198" s="4"/>
     </row>
-    <row r="199" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A199" s="7"/>
       <c r="B199" s="4"/>
       <c r="C199" s="7"/>
@@ -5989,7 +6821,7 @@
       <c r="O199" s="4"/>
       <c r="S199" s="4"/>
     </row>
-    <row r="200" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A200" s="7"/>
       <c r="B200" s="4"/>
       <c r="C200" s="7"/>
@@ -6007,7 +6839,7 @@
       <c r="O200" s="4"/>
       <c r="S200" s="4"/>
     </row>
-    <row r="201" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A201" s="7"/>
       <c r="B201" s="4"/>
       <c r="C201" s="7"/>
@@ -6025,7 +6857,7 @@
       <c r="O201" s="4"/>
       <c r="S201" s="4"/>
     </row>
-    <row r="202" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A202" s="7"/>
       <c r="B202" s="4"/>
       <c r="C202" s="7"/>
@@ -6043,7 +6875,7 @@
       <c r="O202" s="4"/>
       <c r="S202" s="4"/>
     </row>
-    <row r="203" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A203" s="7"/>
       <c r="B203" s="4"/>
       <c r="C203" s="7"/>
@@ -6061,7 +6893,7 @@
       <c r="O203" s="4"/>
       <c r="S203" s="4"/>
     </row>
-    <row r="204" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A204" s="7"/>
       <c r="B204" s="4"/>
       <c r="C204" s="7"/>
@@ -6079,7 +6911,7 @@
       <c r="O204" s="4"/>
       <c r="S204" s="4"/>
     </row>
-    <row r="205" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A205" s="7"/>
       <c r="B205" s="4"/>
       <c r="C205" s="7"/>
@@ -6097,7 +6929,7 @@
       <c r="O205" s="4"/>
       <c r="S205" s="4"/>
     </row>
-    <row r="206" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A206" s="7"/>
       <c r="B206" s="4"/>
       <c r="C206" s="7"/>
@@ -6115,7 +6947,7 @@
       <c r="O206" s="4"/>
       <c r="S206" s="4"/>
     </row>
-    <row r="207" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A207" s="7"/>
       <c r="B207" s="4"/>
       <c r="C207" s="7"/>
@@ -6133,7 +6965,7 @@
       <c r="O207" s="4"/>
       <c r="S207" s="4"/>
     </row>
-    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A208" s="7"/>
       <c r="B208" s="4"/>
       <c r="C208" s="7"/>
@@ -6151,7 +6983,7 @@
       <c r="O208" s="4"/>
       <c r="S208" s="4"/>
     </row>
-    <row r="209" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A209" s="7"/>
       <c r="B209" s="4"/>
       <c r="C209" s="7"/>
@@ -6169,7 +7001,7 @@
       <c r="O209" s="4"/>
       <c r="S209" s="4"/>
     </row>
-    <row r="210" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A210" s="7"/>
       <c r="B210" s="4"/>
       <c r="C210" s="7"/>
@@ -6187,7 +7019,7 @@
       <c r="O210" s="4"/>
       <c r="S210" s="4"/>
     </row>
-    <row r="211" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A211" s="7"/>
       <c r="B211" s="4"/>
       <c r="C211" s="7"/>
@@ -6205,7 +7037,7 @@
       <c r="O211" s="4"/>
       <c r="S211" s="4"/>
     </row>
-    <row r="212" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A212" s="7"/>
       <c r="B212" s="4"/>
       <c r="C212" s="7"/>
@@ -6223,7 +7055,7 @@
       <c r="O212" s="4"/>
       <c r="S212" s="4"/>
     </row>
-    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A213" s="7"/>
       <c r="B213" s="4"/>
       <c r="C213" s="7"/>
@@ -6241,7 +7073,7 @@
       <c r="O213" s="4"/>
       <c r="S213" s="4"/>
     </row>
-    <row r="214" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A214" s="7"/>
       <c r="B214" s="4"/>
       <c r="C214" s="7"/>
@@ -6259,7 +7091,7 @@
       <c r="O214" s="4"/>
       <c r="S214" s="4"/>
     </row>
-    <row r="215" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A215" s="7"/>
       <c r="B215" s="4"/>
       <c r="C215" s="7"/>
@@ -6277,7 +7109,7 @@
       <c r="O215" s="4"/>
       <c r="S215" s="4"/>
     </row>
-    <row r="216" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A216" s="7"/>
       <c r="B216" s="4"/>
       <c r="C216" s="7"/>
@@ -6295,7 +7127,7 @@
       <c r="O216" s="4"/>
       <c r="S216" s="4"/>
     </row>
-    <row r="217" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A217" s="7"/>
       <c r="B217" s="4"/>
       <c r="C217" s="7"/>
@@ -6313,7 +7145,7 @@
       <c r="O217" s="4"/>
       <c r="S217" s="4"/>
     </row>
-    <row r="218" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A218" s="7"/>
       <c r="B218" s="4"/>
       <c r="C218" s="7"/>
@@ -6346,18 +7178,18 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="43.21875" customWidth="1"/>
+    <col min="2" max="2" width="43.25" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
-    <col min="7" max="7" width="42.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" customWidth="1"/>
+    <col min="6" max="6" width="20.625" customWidth="1"/>
+    <col min="7" max="7" width="42.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="24" t="s">
         <v>19</v>
       </c>
@@ -6383,7 +7215,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -6393,7 +7225,7 @@
       <c r="G2" s="26"/>
       <c r="H2" s="26"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="25"/>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -6403,7 +7235,7 @@
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="25"/>
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
@@ -6413,7 +7245,7 @@
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="25"/>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
@@ -6423,7 +7255,7 @@
       <c r="G5" s="25"/>
       <c r="H5" s="25"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="25"/>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -6433,7 +7265,7 @@
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="25"/>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
@@ -6443,7 +7275,7 @@
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="25"/>
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
@@ -6453,7 +7285,7 @@
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="25"/>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
@@ -6463,7 +7295,7 @@
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="25"/>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
@@ -6473,7 +7305,7 @@
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="25"/>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
@@ -6483,7 +7315,7 @@
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="25"/>
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
@@ -6493,7 +7325,7 @@
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="25"/>
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
@@ -6503,7 +7335,7 @@
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="25"/>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
@@ -6513,7 +7345,7 @@
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="25"/>
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
@@ -6523,7 +7355,7 @@
       <c r="G15" s="25"/>
       <c r="H15" s="25"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="25"/>
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
@@ -6533,7 +7365,7 @@
       <c r="G16" s="25"/>
       <c r="H16" s="25"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="25"/>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
@@ -6543,7 +7375,7 @@
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="25"/>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
@@ -6553,7 +7385,7 @@
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="25"/>
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>

</xml_diff>